<commit_message>
first go, works, need to put a tcl UI onto it
</commit_message>
<xml_diff>
--- a/Templates/Template.xlsx
+++ b/Templates/Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scottejames/Projects/DownsmanCheckpoint/Templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{12ED2BE7-F293-A947-A2A0-A9E936500C61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A24EFC57-4669-424C-8922-0E591161F992}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16400" xr2:uid="{94B085BF-E882-0D4F-A724-506E76D0B1FD}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16340" xr2:uid="{94B085BF-E882-0D4F-A724-506E76D0B1FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -83,15 +83,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -99,12 +105,124 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -419,10 +537,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB89E452-D6DB-1348-9495-D19665C78876}">
-  <dimension ref="B2:I6"/>
+  <dimension ref="B2:I27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D6" sqref="D6:I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -453,31 +571,242 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
+    <row r="5" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="2:9" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" s="1" t="s">
         <v>10</v>
       </c>
+    </row>
+    <row r="7" spans="2:9" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="11"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="3"/>
+    </row>
+    <row r="8" spans="2:9" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="13"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="2"/>
+    </row>
+    <row r="9" spans="2:9" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="11"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="3"/>
+    </row>
+    <row r="10" spans="2:9" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="13"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="2"/>
+    </row>
+    <row r="11" spans="2:9" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="11"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="3"/>
+    </row>
+    <row r="12" spans="2:9" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="13"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="2"/>
+    </row>
+    <row r="13" spans="2:9" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="11"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="3"/>
+    </row>
+    <row r="14" spans="2:9" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="13"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="2"/>
+    </row>
+    <row r="15" spans="2:9" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="11"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="3"/>
+    </row>
+    <row r="16" spans="2:9" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="13"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="2"/>
+    </row>
+    <row r="17" spans="2:9" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="11"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="3"/>
+    </row>
+    <row r="18" spans="2:9" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="13"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="2"/>
+    </row>
+    <row r="19" spans="2:9" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="11"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="3"/>
+    </row>
+    <row r="20" spans="2:9" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="13"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="2"/>
+    </row>
+    <row r="21" spans="2:9" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="11"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="3"/>
+    </row>
+    <row r="22" spans="2:9" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="13"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="2"/>
+    </row>
+    <row r="23" spans="2:9" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="11"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="3"/>
+    </row>
+    <row r="24" spans="2:9" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="13"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="2"/>
+    </row>
+    <row r="25" spans="2:9" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="11"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="3"/>
+    </row>
+    <row r="26" spans="2:9" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="13"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="2"/>
+    </row>
+    <row r="27" spans="2:9" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="15"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>